<commit_message>
tried stopwords approach. will investigate further.
</commit_message>
<xml_diff>
--- a/vizegrades.xlsx
+++ b/vizegrades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkkas/Documents/TEZ/Tez/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2197AC62-D189-2B4B-BCE2-5FC44613E66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9223BA-B258-BF40-8488-C4A90F8CF100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cevap1" sheetId="1" r:id="rId1"/>
@@ -1822,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -7997,7 +7997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -8077,7 +8077,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="304" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="224" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>20170808017</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>20190808014</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>20190808023</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20190808024</v>
       </c>
@@ -8261,7 +8261,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>20190808092</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>20195156020</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>20200808005</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="208" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>20200808006</v>
       </c>
@@ -8399,7 +8399,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>20200808009</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>20200808014</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>20200808015</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20200808018</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="224" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>20200808023</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>20200808024</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>20200808030</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>20200808033</v>
       </c>
@@ -8698,7 +8698,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>20200808036</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>20200808038</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>20200808039</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="224" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>20200808040</v>
       </c>
@@ -8813,7 +8813,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>20200808042</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>20200808043</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>20200808044</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>20200808046</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>20200808047</v>
       </c>
@@ -8951,7 +8951,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="208" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>20200808048</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>20200808050</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>20200808051</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>20200808053</v>
       </c>
@@ -9089,7 +9089,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>20200808054</v>
       </c>
@@ -9135,7 +9135,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>20200808059</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="288" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="224" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>20200808060</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>20200808062</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>20200808067</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>20200808070</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>20200808076</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="288" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="208" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>20200808081</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>20200808082</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>20200808504</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="335" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="256" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>20200808605</v>
       </c>
@@ -9503,7 +9503,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>20200808804</v>
       </c>
@@ -9526,7 +9526,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="256" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>20205156018</v>
       </c>
@@ -9572,7 +9572,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="240" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>20210808009</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>20210808019</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="224" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>20210808020</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="320" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="240" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>20210808023</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>20210808047</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>20210808050</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>20210808055</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>20210808062</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>20210808063</v>
       </c>
@@ -9894,7 +9894,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>20210808603</v>
       </c>
@@ -9917,7 +9917,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>20210808604</v>
       </c>
@@ -10009,7 +10009,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>20210808617</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>20210808618</v>
       </c>
@@ -10064,7 +10064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>